<commit_message>
menyesuaikan data cleaning dengan code, memperbarui hasil mae dan rmse
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a c e r\OneDrive\Pictures\Semester 7\TA1\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD307346-07BB-4B26-B847-70538BF495C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB64B57-D3AE-4E8E-B828-CCF2EC4FF5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,9 +618,6 @@
     <t>tv analog, tv digital, kominfo, viral, presiden jokowi</t>
   </si>
   <si>
-    <t>Lmpung Utara</t>
-  </si>
-  <si>
     <t>Kejari Kotabumi, oknum jaksa, narkotika, narkoba</t>
   </si>
   <si>
@@ -643,6 +640,9 @@
   </si>
   <si>
     <t>polres pringsewu, barang bukti, satresnarkoba, sabu, narkoba</t>
+  </si>
+  <si>
+    <t>Lampung Utara</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1041,8 @@
   </sheetPr>
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1073,7 +1073,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="255" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="242.25" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="293.25" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="293.25" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="89.25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="344.25" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="114.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="331.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="102" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="408" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="280.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="280.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="89.25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="369.75" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="306" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="293.25" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="255" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="306" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="229.5" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="293.25" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="306" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="267.75" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="216.75" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="255" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="204" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="191.25" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="242.25" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="255" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>48</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="267.75" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="89.25" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="344.25" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="293.25" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="229.5" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -2167,13 +2167,13 @@
         <v>112</v>
       </c>
       <c r="E56" t="s">
+        <v>204</v>
+      </c>
+      <c r="F56" t="s">
         <v>196</v>
       </c>
-      <c r="F56" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:6" ht="306" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -2190,10 +2190,10 @@
         <v>146</v>
       </c>
       <c r="F57" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="89.25" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="216.75" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -2210,10 +2210,10 @@
         <v>181</v>
       </c>
       <c r="F58" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="255" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -2230,10 +2230,10 @@
         <v>181</v>
       </c>
       <c r="F59" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="89.25" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="255" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -2247,13 +2247,13 @@
         <v>120</v>
       </c>
       <c r="E60" t="s">
+        <v>200</v>
+      </c>
+      <c r="F60" t="s">
         <v>201</v>
       </c>
-      <c r="F60" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:6" ht="293.25" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -2267,10 +2267,10 @@
         <v>122</v>
       </c>
       <c r="E61" t="s">
+        <v>202</v>
+      </c>
+      <c r="F61" t="s">
         <v>203</v>
-      </c>
-      <c r="F61" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.35">

</xml_diff>